<commit_message>
Fill Error Summury worklist
Fill Error Summury worklist and some formatting changes.
</commit_message>
<xml_diff>
--- a/160123_t.xlsx
+++ b/160123_t.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="285" windowWidth="14400" windowHeight="8445" tabRatio="769" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="285" windowWidth="14400" windowHeight="8445" tabRatio="769" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Front Sheet" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Controller log template" sheetId="45" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Error list. Summary'!$A$4:$Q$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Error list. Summary'!$A$4:$J$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Check Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Overall</t>
   </si>
   <si>
-    <t>altk</t>
-  </si>
-  <si>
     <t>Node type</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>v&lt;#DateOf#&gt;</t>
+  </si>
+  <si>
+    <t>v&lt;#Command#&gt;</t>
+  </si>
+  <si>
+    <t>Command(s)</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[Black]0.0%"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,14 +250,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -396,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -415,46 +410,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -465,14 +457,7 @@
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <strike val="0"/>
@@ -512,6 +497,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
       </font>
@@ -557,13 +549,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
       </font>
@@ -595,6 +580,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
       </font>
@@ -633,6 +632,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
       </font>
@@ -671,40 +677,33 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1035,8 +1034,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="23" t="s">
-        <v>25</v>
+      <c r="B1" s="22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="38.25">
@@ -1045,181 +1044,181 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1">
+      <c r="B6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="C6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1">
+      <c r="B7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1">
-      <c r="B6" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" customHeight="1">
-      <c r="B7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="18">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="17">
         <f>SUM(F6:F7)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <f>SUM(G6:G7)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <f>SUM(H6:H7)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="17">
         <f>SUM(I6:I7)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <f>SUM(J6:J7)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="17">
         <f>SUM(F9:J9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21" t="e">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20" t="e">
         <f>F9/K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G10" s="21" t="e">
+      <c r="G10" s="20" t="e">
         <f>G9/K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="21" t="e">
+      <c r="H10" s="20" t="e">
         <f>H9/K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="21" t="e">
+      <c r="I10" s="20" t="e">
         <f>I9/K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="21" t="e">
+      <c r="J10" s="20" t="e">
         <f>J9/K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="21" t="e">
+      <c r="K10" s="20" t="e">
         <f>K9/K9</f>
         <v>#DIV/0!</v>
       </c>
@@ -1263,63 +1262,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    <row r="1" spans="1:10">
+      <c r="A1" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.25">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="20.25">
+      <c r="C10" s="8"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A4:J4">
+    <sortState ref="A5:J8">
+      <sortCondition sortBy="cellColor" ref="D5:D8" dxfId="32"/>
+      <sortCondition sortBy="cellColor" ref="D5:D8" dxfId="31"/>
+      <sortCondition sortBy="cellColor" ref="D5:D8" dxfId="30"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="D5:D243">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH("Critical",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH("Critical",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Major">
+      <formula>NOT(ISERROR(SEARCH("Major",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Minor">
+      <formula>NOT(ISERROR(SEARCH("Minor",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Warning">
+      <formula>NOT(ISERROR(SEARCH("Warning",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Ok">
+      <formula>NOT(ISERROR(SEARCH("Ok",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1329,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1344,13 +1438,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -1362,7 +1456,9 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1387,22 +1483,22 @@
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="11" t="s">
-        <v>39</v>
+      <c r="H5" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -1420,22 +1516,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C240">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Critical">
+    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH("Critical",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="316" operator="containsText" text="Critical">
+    <cfRule type="containsText" dxfId="28" priority="316" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH("Critical",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="317" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="27" priority="317" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="318" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="26" priority="318" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="319" operator="containsText" text="Warning">
+    <cfRule type="containsText" dxfId="25" priority="319" operator="containsText" text="Warning">
       <formula>NOT(ISERROR(SEARCH("Warning",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="320" operator="containsText" text="Ok">
+    <cfRule type="containsText" dxfId="24" priority="320" operator="containsText" text="Ok">
       <formula>NOT(ISERROR(SEARCH("Ok",C5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>